<commit_message>
Excel vezérlés hozzáadása 2
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="B2:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -439,9 +439,14 @@
       <c r="D3" t="n">
         <v>30</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Hibás</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel vezérlés hozzáadása 3
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="B2:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -441,12 +441,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Hibás</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel vezérlés hozzáadása 4
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -394,10 +394,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:G3"/>
+  <dimension ref="B2:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B3" sqref="B3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -442,6 +442,79 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Hibás</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" t="n">
+        <v>70</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n">
+        <v>90</v>
+      </c>
+      <c r="C6" t="n">
+        <v>60</v>
+      </c>
+      <c r="D6" t="n">
+        <v>150</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Hibás</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="34">
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Hibás</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Hibás</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Szorzás, Osztás Minden site alphelyzetbe állítása
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Összeadás" sheetId="1" state="visible" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="B2:G36"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Hibás</t>
         </is>
       </c>
     </row>
@@ -462,7 +462,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -483,12 +483,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Hibás</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -542,8 +542,8 @@
   </sheetPr>
   <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -590,6 +590,11 @@
           <t>Pass</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="n">
@@ -625,6 +630,11 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>Pass</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -661,15 +671,126 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:B3"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F3" sqref="F3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3"/>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bement 1 </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bemenet 2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bemenet 3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pass/Fail</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Üzenet</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D4" t="n">
+        <v>600</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>70</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2101</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Hibás</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n">
+        <v>90</v>
+      </c>
+      <c r="C6" t="n">
+        <v>60</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5400</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -681,15 +802,126 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:B3"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3"/>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bement 1 </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bemenet 2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Bemenet 3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pass/Fail</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Üzenet</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Hibás</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n">
+        <v>90</v>
+      </c>
+      <c r="C6" t="n">
+        <v>60</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>